<commit_message>
added automatization for marks orders
</commit_message>
<xml_diff>
--- a/public/wildberries/new.xlsx
+++ b/public/wildberries/new.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="160">
   <si>
     <t>Номер задания</t>
   </si>
@@ -71,13 +71,13 @@
     <t>Время с момента заказа</t>
   </si>
   <si>
-    <t>WB-GI-37330636</t>
-  </si>
-  <si>
-    <t>11211555650</t>
-  </si>
-  <si>
-    <t>20:24:59 25.04.2023</t>
+    <t>WB-GI-45005734</t>
+  </si>
+  <si>
+    <t>11154949972</t>
+  </si>
+  <si>
+    <t>16:45:50 24.04.2023</t>
   </si>
   <si>
     <t>-</t>
@@ -89,16 +89,16 @@
     <t>0</t>
   </si>
   <si>
-    <t>красный</t>
+    <t>зеленый</t>
   </si>
   <si>
     <t>₽</t>
   </si>
   <si>
-    <t>138871211</t>
-  </si>
-  <si>
-    <t>00-00147126</t>
+    <t>138870993</t>
+  </si>
+  <si>
+    <t>00-00185259</t>
   </si>
   <si>
     <t>Склад</t>
@@ -107,148 +107,331 @@
     <t>Новое</t>
   </si>
   <si>
-    <t>15 ч 14 мин</t>
-  </si>
-  <si>
-    <t>11211285671</t>
-  </si>
-  <si>
-    <t>18:13:38 25.04.2023</t>
+    <t>48 ч 04 мин</t>
+  </si>
+  <si>
+    <t>11154949975</t>
+  </si>
+  <si>
+    <t>11155322006</t>
+  </si>
+  <si>
+    <t>19:58:13 24.04.2023</t>
+  </si>
+  <si>
+    <t>синий</t>
+  </si>
+  <si>
+    <t>138871180</t>
+  </si>
+  <si>
+    <t>00-00190709</t>
+  </si>
+  <si>
+    <t>На сборке</t>
+  </si>
+  <si>
+    <t>44 ч 52 мин</t>
+  </si>
+  <si>
+    <t>11155322014</t>
+  </si>
+  <si>
+    <t>11155874832</t>
+  </si>
+  <si>
+    <t>06:06:36 25.04.2023</t>
   </si>
   <si>
     <t>Наволочка из тенселя 50 х 70</t>
   </si>
   <si>
+    <t>голубой</t>
+  </si>
+  <si>
+    <t>138871447</t>
+  </si>
+  <si>
+    <t>00-00193331</t>
+  </si>
+  <si>
+    <t>34 ч 43 мин</t>
+  </si>
+  <si>
+    <t>11182927640</t>
+  </si>
+  <si>
+    <t>14:07:12 25.04.2023</t>
+  </si>
+  <si>
+    <t>Постельное бельё из бязи 1,5 спальное</t>
+  </si>
+  <si>
+    <t>черный</t>
+  </si>
+  <si>
+    <t>149929992</t>
+  </si>
+  <si>
+    <t>00-00201663</t>
+  </si>
+  <si>
+    <t>26 ч 43 мин</t>
+  </si>
+  <si>
+    <t>11188516914</t>
+  </si>
+  <si>
+    <t>14:17:44 25.04.2023</t>
+  </si>
+  <si>
+    <t>Постельное бельё из сатина 1,5 спальное на резинке 90х200х30</t>
+  </si>
+  <si>
+    <t>светло-розовый</t>
+  </si>
+  <si>
+    <t>157397875</t>
+  </si>
+  <si>
+    <t>00-00203025</t>
+  </si>
+  <si>
+    <t>26 ч 32 мин</t>
+  </si>
+  <si>
+    <t>11154246473</t>
+  </si>
+  <si>
+    <t>12:25:05 24.04.2023</t>
+  </si>
+  <si>
+    <t>Простыня из варёного хлопка на резинке 180х200х20</t>
+  </si>
+  <si>
+    <t>розовый</t>
+  </si>
+  <si>
+    <t>136504358</t>
+  </si>
+  <si>
+    <t>00-00196118</t>
+  </si>
+  <si>
+    <t>52 ч 25 мин</t>
+  </si>
+  <si>
+    <t>11155322005</t>
+  </si>
+  <si>
+    <t>Простыня из сатина 180x220</t>
+  </si>
+  <si>
+    <t>135531353</t>
+  </si>
+  <si>
+    <t>00-00190730</t>
+  </si>
+  <si>
+    <t>11150097369</t>
+  </si>
+  <si>
+    <t>11:29:04 24.04.2023</t>
+  </si>
+  <si>
+    <t>Простыня из сатина 240x260</t>
+  </si>
+  <si>
     <t>белый</t>
   </si>
   <si>
-    <t>138871637</t>
-  </si>
-  <si>
-    <t>00-00182255</t>
-  </si>
-  <si>
-    <t>17 ч 25 мин</t>
-  </si>
-  <si>
-    <t>11211554715</t>
-  </si>
-  <si>
-    <t>20:24:10 25.04.2023</t>
-  </si>
-  <si>
-    <t>Постельное белье из бязи 1,5 спальное</t>
-  </si>
-  <si>
-    <t>голубой</t>
-  </si>
-  <si>
-    <t>141291805</t>
-  </si>
-  <si>
-    <t>00-00186996</t>
-  </si>
-  <si>
-    <t>15 ч 15 мин</t>
-  </si>
-  <si>
-    <t>11211720666</t>
-  </si>
-  <si>
-    <t>23:15:15 25.04.2023</t>
-  </si>
-  <si>
-    <t>Простыня из сатина 150x220</t>
-  </si>
-  <si>
-    <t>136504749</t>
-  </si>
-  <si>
-    <t>00-00146990</t>
-  </si>
-  <si>
-    <t>12 ч 24 мин</t>
-  </si>
-  <si>
-    <t>11211507818</t>
-  </si>
-  <si>
-    <t>19:53:54 25.04.2023</t>
-  </si>
-  <si>
-    <t>Простыня из страйп-сатина на резинке 200x200x40</t>
-  </si>
-  <si>
-    <t>темно-синий</t>
-  </si>
-  <si>
-    <t>157399681</t>
-  </si>
-  <si>
-    <t>00-00203442</t>
-  </si>
-  <si>
-    <t>15 ч 45 мин</t>
-  </si>
-  <si>
-    <t>11211303628</t>
-  </si>
-  <si>
-    <t>18:22:25 25.04.2023</t>
-  </si>
-  <si>
-    <t>Простыня из страйп-сатина на резинке 200x220x20</t>
-  </si>
-  <si>
-    <t>бежевый</t>
-  </si>
-  <si>
-    <t>136503823</t>
-  </si>
-  <si>
-    <t>00-00196986</t>
-  </si>
-  <si>
-    <t>17 ч 17 мин</t>
-  </si>
-  <si>
-    <t>11211303627</t>
-  </si>
-  <si>
-    <t>сиреневый</t>
-  </si>
-  <si>
-    <t>136504461</t>
-  </si>
-  <si>
-    <t>00-00196914</t>
-  </si>
-  <si>
-    <t>11211592662</t>
-  </si>
-  <si>
-    <t>21:01:43 25.04.2023</t>
-  </si>
-  <si>
-    <t>Простыня непромокаемая 180x220</t>
-  </si>
-  <si>
-    <t>135533015</t>
-  </si>
-  <si>
-    <t>00-00197016</t>
-  </si>
-  <si>
-    <t>14 ч 37 мин</t>
-  </si>
-  <si>
-    <t>11211316360</t>
-  </si>
-  <si>
-    <t>18:29:11 25.04.2023</t>
-  </si>
-  <si>
-    <t>17 ч 10 мин</t>
+    <t>135486994</t>
+  </si>
+  <si>
+    <t>00-00147094</t>
+  </si>
+  <si>
+    <t>53 ч 21 мин</t>
+  </si>
+  <si>
+    <t>11156110766</t>
+  </si>
+  <si>
+    <t>07:54:33 25.04.2023</t>
+  </si>
+  <si>
+    <t>Простыня из сатина на резинке 180x200x40</t>
+  </si>
+  <si>
+    <t>148723505</t>
+  </si>
+  <si>
+    <t>00-00201131</t>
+  </si>
+  <si>
+    <t>32 ч 55 мин</t>
+  </si>
+  <si>
+    <t>11154949974</t>
+  </si>
+  <si>
+    <t>Простыня из сатина со швом 280x280</t>
+  </si>
+  <si>
+    <t>135531561</t>
+  </si>
+  <si>
+    <t>00-00191366</t>
+  </si>
+  <si>
+    <t>11149536466</t>
+  </si>
+  <si>
+    <t>10:05:20 24.04.2023</t>
+  </si>
+  <si>
+    <t>Простыня из страйп сатина 200x220</t>
+  </si>
+  <si>
+    <t>136503339</t>
+  </si>
+  <si>
+    <t>00-00097043</t>
+  </si>
+  <si>
+    <t>54 ч 45 мин</t>
+  </si>
+  <si>
+    <t>11156159867</t>
+  </si>
+  <si>
+    <t>08:19:22 25.04.2023</t>
+  </si>
+  <si>
+    <t>Простыня из страйп-сатина 300x300</t>
+  </si>
+  <si>
+    <t>темно-коричневый</t>
+  </si>
+  <si>
+    <t>136505153</t>
+  </si>
+  <si>
+    <t>00-00189047</t>
+  </si>
+  <si>
+    <t>32 ч 31 мин</t>
+  </si>
+  <si>
+    <t>11156004804</t>
+  </si>
+  <si>
+    <t>07:09:43 25.04.2023</t>
+  </si>
+  <si>
+    <t>Простыня из страйп-сатина на резинке 140x200x30</t>
+  </si>
+  <si>
+    <t>коричневый</t>
+  </si>
+  <si>
+    <t>136503606</t>
+  </si>
+  <si>
+    <t>00-00142812</t>
+  </si>
+  <si>
+    <t>33 ч 40 мин</t>
+  </si>
+  <si>
+    <t>11149225207</t>
+  </si>
+  <si>
+    <t>08:05:45 24.04.2023</t>
+  </si>
+  <si>
+    <t>Простыня из страйп-сатина на резинке 180x200x30</t>
+  </si>
+  <si>
+    <t>136504392</t>
+  </si>
+  <si>
+    <t>00-00152880</t>
+  </si>
+  <si>
+    <t>56 ч 44 мин</t>
+  </si>
+  <si>
+    <t>11156160608</t>
+  </si>
+  <si>
+    <t>08:19:42 25.04.2023</t>
+  </si>
+  <si>
+    <t>Простыня из страйп-сатина со швами 300x300</t>
+  </si>
+  <si>
+    <t>136504621</t>
+  </si>
+  <si>
+    <t>00-00189071</t>
+  </si>
+  <si>
+    <t>32 ч 30 мин</t>
+  </si>
+  <si>
+    <t>11154265406</t>
+  </si>
+  <si>
+    <t>12:30:57 24.04.2023</t>
+  </si>
+  <si>
+    <t>Простыня из тенселя на резинке 160х200х20</t>
+  </si>
+  <si>
+    <t>светло-зеленый</t>
+  </si>
+  <si>
+    <t>154176279</t>
+  </si>
+  <si>
+    <t>00-00202198</t>
+  </si>
+  <si>
+    <t>52 ч 19 мин</t>
+  </si>
+  <si>
+    <t>11156110768</t>
+  </si>
+  <si>
+    <t>Простыня из тенселя на резинке 180х200х20</t>
+  </si>
+  <si>
+    <t>154176185</t>
+  </si>
+  <si>
+    <t>00-00194290</t>
+  </si>
+  <si>
+    <t>11148441355</t>
+  </si>
+  <si>
+    <t>20:36:54 23.04.2023</t>
+  </si>
+  <si>
+    <t>Простыня из тенселя на резинке 80х200х40</t>
+  </si>
+  <si>
+    <t>медь</t>
+  </si>
+  <si>
+    <t>154176086</t>
+  </si>
+  <si>
+    <t>00-00202877</t>
+  </si>
+  <si>
+    <t>68 ч 13 мин</t>
   </si>
   <si>
     <t>КИЗ</t>
@@ -257,31 +440,61 @@
     <t>Номер чека</t>
   </si>
   <si>
-    <t>0102900240575796215R)gH=gHP.&amp;cp</t>
-  </si>
-  <si>
-    <t>0102900076995171215WGLSv:.Dl%ii</t>
-  </si>
-  <si>
-    <t>0102900240575789215+icRUIdfUo)!</t>
-  </si>
-  <si>
-    <t>0102900240575802215Em&amp;Pmz(Z+Eq"</t>
-  </si>
-  <si>
-    <t>0102900240575772215i3SojIGQmBkN</t>
-  </si>
-  <si>
-    <t>0102900079606234215E/19PkYi3H&lt;m</t>
-  </si>
-  <si>
-    <t>0102900080889404215E)uTQGplCGj-</t>
-  </si>
-  <si>
-    <t>0102900079991279215D&amp;;d9ZcP8RYx</t>
-  </si>
-  <si>
-    <t>0102900079991279215lCVnZhKPuDqL</t>
+    <t>0102900098420118215JN8,VJYV9xo8</t>
+  </si>
+  <si>
+    <t>0102900098420118215+kEhgqqfY)sE</t>
+  </si>
+  <si>
+    <t>0102900203466956215ns5DIWQufX0?</t>
+  </si>
+  <si>
+    <t>0102900203466956215ecXQP&gt;Mt3wa8</t>
+  </si>
+  <si>
+    <t>01029002405756972151t_&gt;aeZ8TPVo</t>
+  </si>
+  <si>
+    <t>0102900240575741215kXq_TQ2P)bqA</t>
+  </si>
+  <si>
+    <t>0102900240575758215OFJl)X&gt;Ls'B6</t>
+  </si>
+  <si>
+    <t>0102900236620370215USA.X3hggeIF</t>
+  </si>
+  <si>
+    <t>0102900240575680215w_B'tK5lKTz=</t>
+  </si>
+  <si>
+    <t>0102900076825430215GJXkqh4i(Z"*</t>
+  </si>
+  <si>
+    <t>0102900234477877215&gt;9hOPcKH4wlU</t>
+  </si>
+  <si>
+    <t>0102900109735224215tJLK)9"20a2g</t>
+  </si>
+  <si>
+    <t>0102900240575635215K%.i;P4UhT%D</t>
+  </si>
+  <si>
+    <t>01029002359186902155R,t+nakYXeI</t>
+  </si>
+  <si>
+    <t>0102900240575703215at6'PnXDKIN=</t>
+  </si>
+  <si>
+    <t>0102900240575628215qgVjtf5VFamN</t>
+  </si>
+  <si>
+    <t>0102900240575734215y-ifn;odSV:z</t>
+  </si>
+  <si>
+    <t>0102900240575642215j(mozMImF(KD</t>
+  </si>
+  <si>
+    <t>01029002405757102154RG&lt;iT;Ihftv</t>
   </si>
 </sst>
 </file>
@@ -628,10 +841,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R10"/>
+  <dimension ref="A1:R21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R1" sqref="R1"/>
+      <selection activeCell="R14" sqref="R14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -639,7 +852,8 @@
     <col min="1" max="3" width="14" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
     <col min="5" max="5" width="20" customWidth="1"/>
-    <col min="6" max="9" width="10" customWidth="1"/>
+    <col min="6" max="6" width="60.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="10" customWidth="1"/>
     <col min="10" max="10" width="7" customWidth="1"/>
     <col min="11" max="11" width="10" customWidth="1"/>
     <col min="12" max="12" width="15" customWidth="1"/>
@@ -708,40 +922,40 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>790378428</v>
+        <v>787224656</v>
       </c>
       <c r="B2" t="s">
         <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>132</v>
       </c>
       <c r="D2" t="s">
-        <v>32</v>
+        <v>133</v>
       </c>
       <c r="E2" t="s">
         <v>21</v>
       </c>
       <c r="F2" t="s">
-        <v>33</v>
+        <v>134</v>
       </c>
       <c r="G2" t="s">
         <v>23</v>
       </c>
       <c r="H2" t="s">
-        <v>34</v>
+        <v>135</v>
       </c>
       <c r="I2">
-        <v>1060</v>
+        <v>3592</v>
       </c>
       <c r="J2" t="s">
         <v>25</v>
       </c>
       <c r="K2" t="s">
-        <v>35</v>
+        <v>136</v>
       </c>
       <c r="L2" t="s">
-        <v>36</v>
+        <v>137</v>
       </c>
       <c r="M2" t="s">
         <v>28</v>
@@ -759,45 +973,45 @@
         <v>21</v>
       </c>
       <c r="R2" t="s">
-        <v>37</v>
+        <v>138</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>790393811</v>
+        <v>787721210</v>
       </c>
       <c r="B3" t="s">
         <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>58</v>
+        <v>109</v>
       </c>
       <c r="D3" t="s">
-        <v>59</v>
+        <v>110</v>
       </c>
       <c r="E3" t="s">
         <v>21</v>
       </c>
       <c r="F3" t="s">
-        <v>60</v>
+        <v>111</v>
       </c>
       <c r="G3" t="s">
         <v>23</v>
       </c>
       <c r="H3" t="s">
-        <v>61</v>
+        <v>105</v>
       </c>
       <c r="I3">
-        <v>3114</v>
+        <v>2858</v>
       </c>
       <c r="J3" t="s">
         <v>25</v>
       </c>
       <c r="K3" t="s">
-        <v>62</v>
+        <v>112</v>
       </c>
       <c r="L3" t="s">
-        <v>63</v>
+        <v>113</v>
       </c>
       <c r="M3" t="s">
         <v>28</v>
@@ -815,45 +1029,45 @@
         <v>21</v>
       </c>
       <c r="R3" t="s">
-        <v>64</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>790393809</v>
+        <v>787915392</v>
       </c>
       <c r="B4" t="s">
         <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>65</v>
+        <v>89</v>
       </c>
       <c r="D4" t="s">
-        <v>59</v>
+        <v>90</v>
       </c>
       <c r="E4" t="s">
         <v>21</v>
       </c>
       <c r="F4" t="s">
-        <v>60</v>
+        <v>91</v>
       </c>
       <c r="G4" t="s">
         <v>23</v>
       </c>
       <c r="H4" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="I4">
-        <v>3114</v>
+        <v>1990</v>
       </c>
       <c r="J4" t="s">
         <v>25</v>
       </c>
       <c r="K4" t="s">
-        <v>67</v>
+        <v>92</v>
       </c>
       <c r="L4" t="s">
-        <v>68</v>
+        <v>93</v>
       </c>
       <c r="M4" t="s">
         <v>28</v>
@@ -871,45 +1085,45 @@
         <v>21</v>
       </c>
       <c r="R4" t="s">
-        <v>64</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>790405372</v>
+        <v>788050636</v>
       </c>
       <c r="B5" t="s">
         <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D5" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E5" t="s">
         <v>21</v>
       </c>
       <c r="F5" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="G5" t="s">
         <v>23</v>
       </c>
       <c r="H5" t="s">
-        <v>34</v>
+        <v>75</v>
       </c>
       <c r="I5">
-        <v>1824</v>
+        <v>2496</v>
       </c>
       <c r="J5" t="s">
         <v>25</v>
       </c>
       <c r="K5" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="L5" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="M5" t="s">
         <v>28</v>
@@ -927,45 +1141,45 @@
         <v>21</v>
       </c>
       <c r="R5" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>790536352</v>
+        <v>788139091</v>
       </c>
       <c r="B6" t="s">
         <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="D6" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="E6" t="s">
         <v>21</v>
       </c>
       <c r="F6" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="G6" t="s">
         <v>23</v>
       </c>
       <c r="H6" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="I6">
-        <v>4257</v>
+        <v>3936</v>
       </c>
       <c r="J6" t="s">
         <v>25</v>
       </c>
       <c r="K6" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="L6" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="M6" t="s">
         <v>28</v>
@@ -983,45 +1197,45 @@
         <v>21</v>
       </c>
       <c r="R6" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>790571551</v>
+        <v>788148151</v>
       </c>
       <c r="B7" t="s">
         <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>38</v>
+        <v>121</v>
       </c>
       <c r="D7" t="s">
-        <v>39</v>
+        <v>122</v>
       </c>
       <c r="E7" t="s">
         <v>21</v>
       </c>
       <c r="F7" t="s">
-        <v>40</v>
+        <v>123</v>
       </c>
       <c r="G7" t="s">
         <v>23</v>
       </c>
       <c r="H7" t="s">
-        <v>41</v>
+        <v>124</v>
       </c>
       <c r="I7">
-        <v>3286</v>
+        <v>3651</v>
       </c>
       <c r="J7" t="s">
         <v>25</v>
       </c>
       <c r="K7" t="s">
-        <v>42</v>
+        <v>125</v>
       </c>
       <c r="L7" t="s">
-        <v>43</v>
+        <v>126</v>
       </c>
       <c r="M7" t="s">
         <v>28</v>
@@ -1039,12 +1253,12 @@
         <v>21</v>
       </c>
       <c r="R7" t="s">
-        <v>44</v>
+        <v>127</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>790572335</v>
+        <v>788540714</v>
       </c>
       <c r="B8" t="s">
         <v>18</v>
@@ -1100,40 +1314,40 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>790603783</v>
+        <v>788540717</v>
       </c>
       <c r="B9" t="s">
         <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>69</v>
+        <v>31</v>
       </c>
       <c r="D9" t="s">
-        <v>70</v>
+        <v>20</v>
       </c>
       <c r="E9" t="s">
         <v>21</v>
       </c>
       <c r="F9" t="s">
-        <v>71</v>
+        <v>22</v>
       </c>
       <c r="G9" t="s">
         <v>23</v>
       </c>
       <c r="H9" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="I9">
-        <v>1824</v>
+        <v>1066</v>
       </c>
       <c r="J9" t="s">
         <v>25</v>
       </c>
       <c r="K9" t="s">
-        <v>72</v>
+        <v>26</v>
       </c>
       <c r="L9" t="s">
-        <v>73</v>
+        <v>27</v>
       </c>
       <c r="M9" t="s">
         <v>28</v>
@@ -1151,45 +1365,45 @@
         <v>21</v>
       </c>
       <c r="R9" t="s">
-        <v>74</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>790655256</v>
+        <v>788540716</v>
       </c>
       <c r="B10" t="s">
         <v>18</v>
       </c>
       <c r="C10" t="s">
-        <v>45</v>
+        <v>85</v>
       </c>
       <c r="D10" t="s">
-        <v>46</v>
+        <v>20</v>
       </c>
       <c r="E10" t="s">
         <v>21</v>
       </c>
       <c r="F10" t="s">
-        <v>47</v>
+        <v>86</v>
       </c>
       <c r="G10" t="s">
         <v>23</v>
       </c>
       <c r="H10" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="I10">
-        <v>2266</v>
+        <v>3489</v>
       </c>
       <c r="J10" t="s">
         <v>25</v>
       </c>
       <c r="K10" t="s">
-        <v>48</v>
+        <v>87</v>
       </c>
       <c r="L10" t="s">
-        <v>49</v>
+        <v>88</v>
       </c>
       <c r="M10" t="s">
         <v>28</v>
@@ -1207,11 +1421,627 @@
         <v>21</v>
       </c>
       <c r="R10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>788846726</v>
+      </c>
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11" t="s">
+        <v>23</v>
+      </c>
+      <c r="H11" t="s">
+        <v>34</v>
+      </c>
+      <c r="I11">
+        <v>1093.99</v>
+      </c>
+      <c r="J11" t="s">
+        <v>25</v>
+      </c>
+      <c r="K11" t="s">
+        <v>35</v>
+      </c>
+      <c r="L11" t="s">
+        <v>36</v>
+      </c>
+      <c r="M11" t="s">
+        <v>28</v>
+      </c>
+      <c r="N11" t="s">
+        <v>37</v>
+      </c>
+      <c r="O11" t="s">
+        <v>21</v>
+      </c>
+      <c r="P11" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>21</v>
+      </c>
+      <c r="R11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>788846734</v>
+      </c>
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" t="s">
+        <v>22</v>
+      </c>
+      <c r="G12" t="s">
+        <v>23</v>
+      </c>
+      <c r="H12" t="s">
+        <v>34</v>
+      </c>
+      <c r="I12">
+        <v>1093.99</v>
+      </c>
+      <c r="J12" t="s">
+        <v>25</v>
+      </c>
+      <c r="K12" t="s">
+        <v>35</v>
+      </c>
+      <c r="L12" t="s">
+        <v>36</v>
+      </c>
+      <c r="M12" t="s">
+        <v>28</v>
+      </c>
+      <c r="N12" t="s">
+        <v>37</v>
+      </c>
+      <c r="O12" t="s">
+        <v>21</v>
+      </c>
+      <c r="P12" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>21</v>
+      </c>
+      <c r="R12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>788846725</v>
+      </c>
+      <c r="B13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" t="s">
+        <v>68</v>
+      </c>
+      <c r="D13" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13" t="s">
+        <v>69</v>
+      </c>
+      <c r="G13" t="s">
+        <v>23</v>
+      </c>
+      <c r="H13" t="s">
+        <v>34</v>
+      </c>
+      <c r="I13">
+        <v>2372.9899999999998</v>
+      </c>
+      <c r="J13" t="s">
+        <v>25</v>
+      </c>
+      <c r="K13" t="s">
+        <v>70</v>
+      </c>
+      <c r="L13" t="s">
+        <v>71</v>
+      </c>
+      <c r="M13" t="s">
+        <v>28</v>
+      </c>
+      <c r="N13" t="s">
+        <v>37</v>
+      </c>
+      <c r="O13" t="s">
+        <v>21</v>
+      </c>
+      <c r="P13" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>21</v>
+      </c>
+      <c r="R13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>789198469</v>
+      </c>
+      <c r="B14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14" t="s">
+        <v>21</v>
+      </c>
+      <c r="F14" t="s">
+        <v>42</v>
+      </c>
+      <c r="G14" t="s">
+        <v>23</v>
+      </c>
+      <c r="H14" t="s">
+        <v>43</v>
+      </c>
+      <c r="I14">
+        <v>1028</v>
+      </c>
+      <c r="J14" t="s">
+        <v>25</v>
+      </c>
+      <c r="K14" t="s">
+        <v>44</v>
+      </c>
+      <c r="L14" t="s">
+        <v>45</v>
+      </c>
+      <c r="M14" t="s">
+        <v>28</v>
+      </c>
+      <c r="N14" t="s">
+        <v>29</v>
+      </c>
+      <c r="O14" t="s">
+        <v>21</v>
+      </c>
+      <c r="P14" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>21</v>
+      </c>
+      <c r="R14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>789297225</v>
+      </c>
+      <c r="B15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" t="s">
+        <v>102</v>
+      </c>
+      <c r="D15" t="s">
+        <v>103</v>
+      </c>
+      <c r="E15" t="s">
+        <v>21</v>
+      </c>
+      <c r="F15" t="s">
+        <v>104</v>
+      </c>
+      <c r="G15" t="s">
+        <v>23</v>
+      </c>
+      <c r="H15" t="s">
+        <v>105</v>
+      </c>
+      <c r="I15">
+        <v>2553</v>
+      </c>
+      <c r="J15" t="s">
+        <v>25</v>
+      </c>
+      <c r="K15" t="s">
+        <v>106</v>
+      </c>
+      <c r="L15" t="s">
+        <v>107</v>
+      </c>
+      <c r="M15" t="s">
+        <v>28</v>
+      </c>
+      <c r="N15" t="s">
+        <v>29</v>
+      </c>
+      <c r="O15" t="s">
+        <v>21</v>
+      </c>
+      <c r="P15" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>21</v>
+      </c>
+      <c r="R15" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>789377823</v>
+      </c>
+      <c r="B16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" t="s">
+        <v>79</v>
+      </c>
+      <c r="D16" t="s">
+        <v>80</v>
+      </c>
+      <c r="E16" t="s">
+        <v>21</v>
+      </c>
+      <c r="F16" t="s">
+        <v>81</v>
+      </c>
+      <c r="G16" t="s">
+        <v>23</v>
+      </c>
+      <c r="H16" t="s">
+        <v>64</v>
+      </c>
+      <c r="I16">
+        <v>3666</v>
+      </c>
+      <c r="J16" t="s">
+        <v>25</v>
+      </c>
+      <c r="K16" t="s">
+        <v>82</v>
+      </c>
+      <c r="L16" t="s">
+        <v>83</v>
+      </c>
+      <c r="M16" t="s">
+        <v>28</v>
+      </c>
+      <c r="N16" t="s">
+        <v>29</v>
+      </c>
+      <c r="O16" t="s">
+        <v>21</v>
+      </c>
+      <c r="P16" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>21</v>
+      </c>
+      <c r="R16" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>789377821</v>
+      </c>
+      <c r="B17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" t="s">
+        <v>128</v>
+      </c>
+      <c r="D17" t="s">
+        <v>80</v>
+      </c>
+      <c r="E17" t="s">
+        <v>21</v>
+      </c>
+      <c r="F17" t="s">
+        <v>129</v>
+      </c>
+      <c r="G17" t="s">
+        <v>23</v>
+      </c>
+      <c r="H17" t="s">
+        <v>64</v>
+      </c>
+      <c r="I17">
+        <v>4054</v>
+      </c>
+      <c r="J17" t="s">
+        <v>25</v>
+      </c>
+      <c r="K17" t="s">
+        <v>130</v>
+      </c>
+      <c r="L17" t="s">
+        <v>131</v>
+      </c>
+      <c r="M17" t="s">
+        <v>28</v>
+      </c>
+      <c r="N17" t="s">
+        <v>29</v>
+      </c>
+      <c r="O17" t="s">
+        <v>21</v>
+      </c>
+      <c r="P17" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>21</v>
+      </c>
+      <c r="R17" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>789418440</v>
+      </c>
+      <c r="B18" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" t="s">
+        <v>95</v>
+      </c>
+      <c r="D18" t="s">
+        <v>96</v>
+      </c>
+      <c r="E18" t="s">
+        <v>21</v>
+      </c>
+      <c r="F18" t="s">
+        <v>97</v>
+      </c>
+      <c r="G18" t="s">
+        <v>23</v>
+      </c>
+      <c r="H18" t="s">
+        <v>98</v>
+      </c>
+      <c r="I18">
+        <v>3305</v>
+      </c>
+      <c r="J18" t="s">
+        <v>25</v>
+      </c>
+      <c r="K18" t="s">
+        <v>99</v>
+      </c>
+      <c r="L18" t="s">
+        <v>100</v>
+      </c>
+      <c r="M18" t="s">
+        <v>28</v>
+      </c>
+      <c r="N18" t="s">
+        <v>29</v>
+      </c>
+      <c r="O18" t="s">
+        <v>21</v>
+      </c>
+      <c r="P18" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>21</v>
+      </c>
+      <c r="R18" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>789419047</v>
+      </c>
+      <c r="B19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" t="s">
+        <v>115</v>
+      </c>
+      <c r="D19" t="s">
+        <v>116</v>
+      </c>
+      <c r="E19" t="s">
+        <v>21</v>
+      </c>
+      <c r="F19" t="s">
+        <v>117</v>
+      </c>
+      <c r="G19" t="s">
+        <v>23</v>
+      </c>
+      <c r="H19" t="s">
+        <v>64</v>
+      </c>
+      <c r="I19">
+        <v>3929</v>
+      </c>
+      <c r="J19" t="s">
+        <v>25</v>
+      </c>
+      <c r="K19" t="s">
+        <v>118</v>
+      </c>
+      <c r="L19" t="s">
+        <v>119</v>
+      </c>
+      <c r="M19" t="s">
+        <v>28</v>
+      </c>
+      <c r="N19" t="s">
+        <v>29</v>
+      </c>
+      <c r="O19" t="s">
+        <v>21</v>
+      </c>
+      <c r="P19" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>21</v>
+      </c>
+      <c r="R19" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>789975578</v>
+      </c>
+      <c r="B20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" t="s">
+        <v>47</v>
+      </c>
+      <c r="D20" t="s">
+        <v>48</v>
+      </c>
+      <c r="E20" t="s">
+        <v>21</v>
+      </c>
+      <c r="F20" t="s">
+        <v>49</v>
+      </c>
+      <c r="G20" t="s">
+        <v>23</v>
+      </c>
+      <c r="H20" t="s">
         <v>50</v>
       </c>
+      <c r="I20">
+        <v>2963</v>
+      </c>
+      <c r="J20" t="s">
+        <v>25</v>
+      </c>
+      <c r="K20" t="s">
+        <v>51</v>
+      </c>
+      <c r="L20" t="s">
+        <v>52</v>
+      </c>
+      <c r="M20" t="s">
+        <v>28</v>
+      </c>
+      <c r="N20" t="s">
+        <v>29</v>
+      </c>
+      <c r="O20" t="s">
+        <v>21</v>
+      </c>
+      <c r="P20" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>21</v>
+      </c>
+      <c r="R20" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>789991695</v>
+      </c>
+      <c r="B21" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" t="s">
+        <v>54</v>
+      </c>
+      <c r="D21" t="s">
+        <v>55</v>
+      </c>
+      <c r="E21" t="s">
+        <v>21</v>
+      </c>
+      <c r="F21" t="s">
+        <v>56</v>
+      </c>
+      <c r="G21" t="s">
+        <v>23</v>
+      </c>
+      <c r="H21" t="s">
+        <v>57</v>
+      </c>
+      <c r="I21">
+        <v>6854</v>
+      </c>
+      <c r="J21" t="s">
+        <v>25</v>
+      </c>
+      <c r="K21" t="s">
+        <v>58</v>
+      </c>
+      <c r="L21" t="s">
+        <v>59</v>
+      </c>
+      <c r="M21" t="s">
+        <v>28</v>
+      </c>
+      <c r="N21" t="s">
+        <v>29</v>
+      </c>
+      <c r="O21" t="s">
+        <v>21</v>
+      </c>
+      <c r="P21" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>21</v>
+      </c>
+      <c r="R21" t="s">
+        <v>60</v>
+      </c>
     </row>
   </sheetData>
-  <sortState ref="A2:R10">
+  <sortState ref="A2:R21">
     <sortCondition descending="1" ref="R1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1220,7 +2050,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1239,109 +2069,219 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>78</v>
+        <v>139</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>79</v>
+        <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>790572335</v>
+        <v>788540714</v>
       </c>
       <c r="B2">
-        <v>11211555650</v>
+        <v>11154949972</v>
       </c>
       <c r="C2" t="s">
-        <v>80</v>
+        <v>141</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>790378428</v>
+        <v>788540717</v>
       </c>
       <c r="B3">
-        <v>11211285671</v>
+        <v>11154949975</v>
       </c>
       <c r="C3" t="s">
-        <v>81</v>
+        <v>142</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>790571551</v>
+        <v>788846726</v>
       </c>
       <c r="B4">
-        <v>11211554715</v>
+        <v>11155322006</v>
       </c>
       <c r="C4" t="s">
-        <v>82</v>
+        <v>143</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>790655256</v>
+        <v>788846734</v>
       </c>
       <c r="B5">
-        <v>11211720666</v>
+        <v>11155322014</v>
       </c>
       <c r="C5" t="s">
-        <v>83</v>
+        <v>144</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>790536352</v>
+        <v>789198469</v>
       </c>
       <c r="B6">
-        <v>11211507818</v>
+        <v>11155874832</v>
       </c>
       <c r="C6" t="s">
-        <v>84</v>
+        <v>145</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>790393811</v>
+        <v>789975578</v>
       </c>
       <c r="B7">
-        <v>11211303628</v>
+        <v>11182927640</v>
       </c>
       <c r="C7" t="s">
-        <v>85</v>
+        <v>146</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>790393809</v>
+        <v>789991695</v>
       </c>
       <c r="B8">
-        <v>11211303627</v>
+        <v>11188516914</v>
       </c>
       <c r="C8" t="s">
-        <v>86</v>
+        <v>147</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>790603783</v>
+        <v>788139091</v>
       </c>
       <c r="B9">
-        <v>11211592662</v>
+        <v>11154246473</v>
       </c>
       <c r="C9" t="s">
-        <v>87</v>
+        <v>148</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>790405372</v>
+        <v>788846725</v>
       </c>
       <c r="B10">
-        <v>11211316360</v>
+        <v>11155322005</v>
       </c>
       <c r="C10" t="s">
-        <v>88</v>
+        <v>149</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>788050636</v>
+      </c>
+      <c r="B11">
+        <v>11150097369</v>
+      </c>
+      <c r="C11" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>789377823</v>
+      </c>
+      <c r="B12">
+        <v>11156110766</v>
+      </c>
+      <c r="C12" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>788540716</v>
+      </c>
+      <c r="B13">
+        <v>11154949974</v>
+      </c>
+      <c r="C13" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>787915392</v>
+      </c>
+      <c r="B14">
+        <v>11149536466</v>
+      </c>
+      <c r="C14" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>789418440</v>
+      </c>
+      <c r="B15">
+        <v>11156159867</v>
+      </c>
+      <c r="C15" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>789297225</v>
+      </c>
+      <c r="B16">
+        <v>11156004804</v>
+      </c>
+      <c r="C16" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>787721210</v>
+      </c>
+      <c r="B17">
+        <v>11149225207</v>
+      </c>
+      <c r="C17" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>789419047</v>
+      </c>
+      <c r="B18">
+        <v>11156160608</v>
+      </c>
+      <c r="C18" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>788148151</v>
+      </c>
+      <c r="B19">
+        <v>11154265406</v>
+      </c>
+      <c r="C19" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>789377821</v>
+      </c>
+      <c r="B20">
+        <v>11156110768</v>
+      </c>
+      <c r="C20" t="s">
+        <v>159</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update import file creating proccess
</commit_message>
<xml_diff>
--- a/public/wildberries/new.xlsx
+++ b/public/wildberries/new.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="96">
   <si>
     <t>№ задания</t>
   </si>
@@ -76,37 +76,31 @@
     <t>Время с момента заказа</t>
   </si>
   <si>
-    <t>WB-GI-54790370</t>
-  </si>
-  <si>
-    <t>13716935806</t>
-  </si>
-  <si>
     <t/>
   </si>
   <si>
-    <t>17:06:20 10.08.2023</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
-    <t>225 Молочный</t>
+    <t>15:42:02 14.08.2023</t>
+  </si>
+  <si>
+    <t>Наволочка из тенселя 40 х 60</t>
   </si>
   <si>
     <t>0</t>
   </si>
   <si>
-    <t>белый</t>
+    <t>голубой</t>
   </si>
   <si>
     <t>₽</t>
   </si>
   <si>
-    <t>133388629</t>
-  </si>
-  <si>
-    <t>00-00195497</t>
+    <t>154170373</t>
+  </si>
+  <si>
+    <t>00-00201723</t>
   </si>
   <si>
     <t>Склад</t>
@@ -115,79 +109,199 @@
     <t>Новое</t>
   </si>
   <si>
-    <t>13 ч 04 мин</t>
-  </si>
-  <si>
-    <t>13717152117</t>
-  </si>
-  <si>
-    <t>18:25:08 10.08.2023</t>
-  </si>
-  <si>
-    <t>Наволочка из варёного хлопка 50 х 70</t>
-  </si>
-  <si>
-    <t>138871467</t>
-  </si>
-  <si>
-    <t>00-00195482</t>
-  </si>
-  <si>
-    <t>11 ч 45 мин</t>
-  </si>
-  <si>
-    <t>13717152116</t>
-  </si>
-  <si>
-    <t>13717397837</t>
-  </si>
-  <si>
-    <t>19:43:02 10.08.2023</t>
+    <t>16 ч 57 мин</t>
+  </si>
+  <si>
+    <t>17:52:42 14.08.2023</t>
+  </si>
+  <si>
+    <t>Пододеяльник из страйп-сатина 200x200</t>
+  </si>
+  <si>
+    <t>желтый</t>
+  </si>
+  <si>
+    <t>138888761</t>
+  </si>
+  <si>
+    <t>00-00190791</t>
+  </si>
+  <si>
+    <t>14 ч 46 мин</t>
+  </si>
+  <si>
+    <t>синий</t>
+  </si>
+  <si>
+    <t>138889378</t>
+  </si>
+  <si>
+    <t>00-00185879</t>
+  </si>
+  <si>
+    <t>19:26:24 14.08.2023</t>
+  </si>
+  <si>
+    <t>4217 Бежевый</t>
+  </si>
+  <si>
+    <t>бежевый</t>
+  </si>
+  <si>
+    <t>129494675</t>
+  </si>
+  <si>
+    <t>00-00191055</t>
+  </si>
+  <si>
+    <t>13 ч 13 мин</t>
+  </si>
+  <si>
+    <t>19:40:23 14.08.2023</t>
+  </si>
+  <si>
+    <t>Постельное бельё из страйп сатина 1,5 спальное 120х200х30</t>
+  </si>
+  <si>
+    <t>148721787</t>
+  </si>
+  <si>
+    <t>00-00186956</t>
+  </si>
+  <si>
+    <t>12 ч 59 мин</t>
+  </si>
+  <si>
+    <t>20:20:19 14.08.2023</t>
+  </si>
+  <si>
+    <t>Наволочка из тенселя 60 х 60</t>
+  </si>
+  <si>
+    <t>черный</t>
+  </si>
+  <si>
+    <t>138871656</t>
+  </si>
+  <si>
+    <t>00-00193246</t>
+  </si>
+  <si>
+    <t>12 ч 19 мин</t>
+  </si>
+  <si>
+    <t>21:21:19 14.08.2023</t>
   </si>
   <si>
     <t>Наволочка из страйп-сатина 50 х 70</t>
   </si>
   <si>
+    <t>138871098</t>
+  </si>
+  <si>
+    <t>00-00190786</t>
+  </si>
+  <si>
+    <t>11 ч 18 мин</t>
+  </si>
+  <si>
+    <t>22:22:53 14.08.2023</t>
+  </si>
+  <si>
+    <t>Простыня из тенселя 300x300</t>
+  </si>
+  <si>
+    <t>136535179</t>
+  </si>
+  <si>
+    <t>00-00193907</t>
+  </si>
+  <si>
+    <t>10 ч 16 мин</t>
+  </si>
+  <si>
+    <t>23:27:14 14.08.2023</t>
+  </si>
+  <si>
+    <t>Наволочка из сатина 40 х 40</t>
+  </si>
+  <si>
+    <t>148720131</t>
+  </si>
+  <si>
+    <t>00-00200984</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 9 ч 12 мин</t>
+  </si>
+  <si>
+    <t>00:25:32 15.08.2023</t>
+  </si>
+  <si>
+    <t>Постельное бельё из страйп сатина 2 спальное 140х200х30</t>
+  </si>
+  <si>
     <t>темно-серый</t>
   </si>
   <si>
-    <t>138871416</t>
-  </si>
-  <si>
-    <t>00-00123649</t>
-  </si>
-  <si>
-    <t>10 ч 27 мин</t>
-  </si>
-  <si>
-    <t>13717397839</t>
-  </si>
-  <si>
-    <t>13717397838</t>
-  </si>
-  <si>
-    <t>Пододеяльник из страйп-сатина 150x200</t>
-  </si>
-  <si>
-    <t>серый</t>
-  </si>
-  <si>
-    <t>138889212</t>
-  </si>
-  <si>
-    <t>00-00185891</t>
-  </si>
-  <si>
-    <t>13717397836</t>
-  </si>
-  <si>
-    <t>Простыня из варёного хлопка 180x220</t>
-  </si>
-  <si>
-    <t>136503593</t>
-  </si>
-  <si>
-    <t>00-00195518</t>
+    <t>149929895</t>
+  </si>
+  <si>
+    <t>00-00201399</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 8 ч 14 мин</t>
+  </si>
+  <si>
+    <t>08:20:16 15.08.2023</t>
+  </si>
+  <si>
+    <t>Наволочка из тенселя 70 х 70</t>
+  </si>
+  <si>
+    <t>зеленый</t>
+  </si>
+  <si>
+    <t>138871687</t>
+  </si>
+  <si>
+    <t>00-00193715</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0 ч 19 мин</t>
+  </si>
+  <si>
+    <t>08:20:44 15.08.2023</t>
+  </si>
+  <si>
+    <t>Матрас ватный тик с бортом 110x190</t>
+  </si>
+  <si>
+    <t>светло-серый</t>
+  </si>
+  <si>
+    <t>135932345</t>
+  </si>
+  <si>
+    <t>00-00150333</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0 ч 18 мин</t>
+  </si>
+  <si>
+    <t>08:21:58 15.08.2023</t>
+  </si>
+  <si>
+    <t>Пододеяльник из тенселя 200x220</t>
+  </si>
+  <si>
+    <t>138889659</t>
+  </si>
+  <si>
+    <t>00-00193720</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0 ч 17 мин</t>
   </si>
 </sst>
 </file>
@@ -534,7 +648,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T8"/>
+  <dimension ref="A1:T18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -620,7 +734,7 @@
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>981700590</v>
+        <v>989683353</v>
       </c>
       <c r="B2" t="s">
         <v>20</v>
@@ -629,431 +743,1051 @@
         <v>21</v>
       </c>
       <c r="D2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" t="s">
         <v>22</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" t="s">
         <v>23</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>24</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>25</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J2">
+        <v>997</v>
+      </c>
+      <c r="K2" t="s">
         <v>26</v>
       </c>
-      <c r="I2" t="s">
+      <c r="L2" t="s">
         <v>27</v>
       </c>
-      <c r="J2">
-        <v>6171</v>
-      </c>
-      <c r="K2" t="s">
+      <c r="M2" t="s">
         <v>28</v>
       </c>
-      <c r="L2" t="s">
+      <c r="N2" t="s">
         <v>29</v>
       </c>
-      <c r="M2" t="s">
+      <c r="O2" t="s">
         <v>30</v>
       </c>
-      <c r="N2" t="s">
+      <c r="P2" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>21</v>
+      </c>
+      <c r="R2" t="s">
+        <v>21</v>
+      </c>
+      <c r="S2" t="s">
+        <v>21</v>
+      </c>
+      <c r="T2" t="s">
         <v>31</v>
-      </c>
-      <c r="O2" t="s">
-        <v>32</v>
-      </c>
-      <c r="P2" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>24</v>
-      </c>
-      <c r="R2" t="s">
-        <v>24</v>
-      </c>
-      <c r="S2" t="s">
-        <v>24</v>
-      </c>
-      <c r="T2" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>981864062</v>
+        <v>989972672</v>
       </c>
       <c r="B3" t="s">
         <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="D3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" t="s">
+        <v>34</v>
+      </c>
+      <c r="J3">
+        <v>3387</v>
+      </c>
+      <c r="K3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L3" t="s">
         <v>35</v>
       </c>
-      <c r="F3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="M3" t="s">
         <v>36</v>
       </c>
-      <c r="H3" t="s">
-        <v>26</v>
-      </c>
-      <c r="I3" t="s">
-        <v>27</v>
-      </c>
-      <c r="J3">
-        <v>964</v>
-      </c>
-      <c r="K3" t="s">
-        <v>28</v>
-      </c>
-      <c r="L3" t="s">
+      <c r="N3" t="s">
+        <v>29</v>
+      </c>
+      <c r="O3" t="s">
+        <v>30</v>
+      </c>
+      <c r="P3" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>21</v>
+      </c>
+      <c r="R3" t="s">
+        <v>21</v>
+      </c>
+      <c r="S3" t="s">
+        <v>21</v>
+      </c>
+      <c r="T3" t="s">
         <v>37</v>
-      </c>
-      <c r="M3" t="s">
-        <v>38</v>
-      </c>
-      <c r="N3" t="s">
-        <v>31</v>
-      </c>
-      <c r="O3" t="s">
-        <v>32</v>
-      </c>
-      <c r="P3" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>24</v>
-      </c>
-      <c r="R3" t="s">
-        <v>24</v>
-      </c>
-      <c r="S3" t="s">
-        <v>24</v>
-      </c>
-      <c r="T3" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>981864063</v>
+        <v>989972674</v>
       </c>
       <c r="B4" t="s">
         <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="D4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H4" t="s">
         <v>24</v>
       </c>
-      <c r="G4" t="s">
-        <v>36</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
+        <v>38</v>
+      </c>
+      <c r="J4">
+        <v>3387</v>
+      </c>
+      <c r="K4" t="s">
         <v>26</v>
       </c>
-      <c r="I4" t="s">
-        <v>27</v>
-      </c>
-      <c r="J4">
-        <v>964</v>
-      </c>
-      <c r="K4" t="s">
-        <v>28</v>
-      </c>
       <c r="L4" t="s">
+        <v>39</v>
+      </c>
+      <c r="M4" t="s">
+        <v>40</v>
+      </c>
+      <c r="N4" t="s">
+        <v>29</v>
+      </c>
+      <c r="O4" t="s">
+        <v>30</v>
+      </c>
+      <c r="P4" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>21</v>
+      </c>
+      <c r="R4" t="s">
+        <v>21</v>
+      </c>
+      <c r="S4" t="s">
+        <v>21</v>
+      </c>
+      <c r="T4" t="s">
         <v>37</v>
-      </c>
-      <c r="M4" t="s">
-        <v>38</v>
-      </c>
-      <c r="N4" t="s">
-        <v>31</v>
-      </c>
-      <c r="O4" t="s">
-        <v>32</v>
-      </c>
-      <c r="P4" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>24</v>
-      </c>
-      <c r="R4" t="s">
-        <v>24</v>
-      </c>
-      <c r="S4" t="s">
-        <v>24</v>
-      </c>
-      <c r="T4" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>982016009</v>
+        <v>990176657</v>
       </c>
       <c r="B5" t="s">
         <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>54</v>
+        <v>21</v>
       </c>
       <c r="D5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" t="s">
         <v>42</v>
       </c>
-      <c r="F5" t="s">
+      <c r="H5" t="s">
         <v>24</v>
       </c>
-      <c r="G5" t="s">
-        <v>55</v>
-      </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
+        <v>43</v>
+      </c>
+      <c r="J5">
+        <v>9079</v>
+      </c>
+      <c r="K5" t="s">
         <v>26</v>
       </c>
-      <c r="I5" t="s">
-        <v>27</v>
-      </c>
-      <c r="J5">
-        <v>2273</v>
-      </c>
-      <c r="K5" t="s">
-        <v>28</v>
-      </c>
       <c r="L5" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="M5" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="N5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="O5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="P5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="Q5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="R5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="S5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="T5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>982016010</v>
+        <v>990206981</v>
       </c>
       <c r="B6" t="s">
         <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="D6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E6" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="F6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" t="s">
+        <v>48</v>
+      </c>
+      <c r="H6" t="s">
         <v>24</v>
       </c>
-      <c r="G6" t="s">
-        <v>43</v>
-      </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
+        <v>25</v>
+      </c>
+      <c r="J6">
+        <v>5435</v>
+      </c>
+      <c r="K6" t="s">
         <v>26</v>
       </c>
-      <c r="I6" t="s">
-        <v>44</v>
-      </c>
-      <c r="J6">
-        <v>871</v>
-      </c>
-      <c r="K6" t="s">
-        <v>28</v>
-      </c>
       <c r="L6" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="M6" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="N6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="O6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="P6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="Q6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="R6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="S6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="T6" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>982016011</v>
+        <v>990291271</v>
       </c>
       <c r="B7" t="s">
         <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>49</v>
+        <v>21</v>
       </c>
       <c r="D7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E7" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="F7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" t="s">
+        <v>53</v>
+      </c>
+      <c r="H7" t="s">
         <v>24</v>
       </c>
-      <c r="G7" t="s">
-        <v>50</v>
-      </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
+        <v>54</v>
+      </c>
+      <c r="J7">
+        <v>1129</v>
+      </c>
+      <c r="K7" t="s">
         <v>26</v>
       </c>
-      <c r="I7" t="s">
-        <v>51</v>
-      </c>
-      <c r="J7">
-        <v>2673</v>
-      </c>
-      <c r="K7" t="s">
-        <v>28</v>
-      </c>
       <c r="L7" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="M7" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="N7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="O7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="P7" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="Q7" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="R7" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="S7" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="T7" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>982016012</v>
+        <v>990427867</v>
       </c>
       <c r="B8" t="s">
         <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>48</v>
+        <v>21</v>
       </c>
       <c r="D8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E8" t="s">
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="F8" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" t="s">
+        <v>59</v>
+      </c>
+      <c r="H8" t="s">
         <v>24</v>
       </c>
-      <c r="G8" t="s">
+      <c r="I8" t="s">
+        <v>34</v>
+      </c>
+      <c r="J8">
+        <v>934</v>
+      </c>
+      <c r="K8" t="s">
+        <v>26</v>
+      </c>
+      <c r="L8" t="s">
+        <v>60</v>
+      </c>
+      <c r="M8" t="s">
+        <v>61</v>
+      </c>
+      <c r="N8" t="s">
+        <v>29</v>
+      </c>
+      <c r="O8" t="s">
+        <v>30</v>
+      </c>
+      <c r="P8" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>21</v>
+      </c>
+      <c r="R8" t="s">
+        <v>21</v>
+      </c>
+      <c r="S8" t="s">
+        <v>21</v>
+      </c>
+      <c r="T8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>990561093</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" t="s">
+        <v>63</v>
+      </c>
+      <c r="F9" t="s">
+        <v>21</v>
+      </c>
+      <c r="G9" t="s">
+        <v>64</v>
+      </c>
+      <c r="H9" t="s">
+        <v>24</v>
+      </c>
+      <c r="I9" t="s">
+        <v>20</v>
+      </c>
+      <c r="J9">
+        <v>4841</v>
+      </c>
+      <c r="K9" t="s">
+        <v>26</v>
+      </c>
+      <c r="L9" t="s">
+        <v>65</v>
+      </c>
+      <c r="M9" t="s">
+        <v>66</v>
+      </c>
+      <c r="N9" t="s">
+        <v>29</v>
+      </c>
+      <c r="O9" t="s">
+        <v>30</v>
+      </c>
+      <c r="P9" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>21</v>
+      </c>
+      <c r="R9" t="s">
+        <v>21</v>
+      </c>
+      <c r="S9" t="s">
+        <v>21</v>
+      </c>
+      <c r="T9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>990673148</v>
+      </c>
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" t="s">
+        <v>68</v>
+      </c>
+      <c r="F10" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10" t="s">
+        <v>69</v>
+      </c>
+      <c r="H10" t="s">
+        <v>24</v>
+      </c>
+      <c r="I10" t="s">
         <v>43</v>
       </c>
-      <c r="H8" t="s">
+      <c r="J10">
+        <v>936</v>
+      </c>
+      <c r="K10" t="s">
         <v>26</v>
       </c>
-      <c r="I8" t="s">
-        <v>44</v>
-      </c>
-      <c r="J8">
-        <v>871</v>
-      </c>
-      <c r="K8" t="s">
-        <v>28</v>
-      </c>
-      <c r="L8" t="s">
-        <v>45</v>
-      </c>
-      <c r="M8" t="s">
-        <v>46</v>
-      </c>
-      <c r="N8" t="s">
-        <v>31</v>
-      </c>
-      <c r="O8" t="s">
-        <v>32</v>
-      </c>
-      <c r="P8" t="s">
+      <c r="L10" t="s">
+        <v>70</v>
+      </c>
+      <c r="M10" t="s">
+        <v>71</v>
+      </c>
+      <c r="N10" t="s">
+        <v>29</v>
+      </c>
+      <c r="O10" t="s">
+        <v>30</v>
+      </c>
+      <c r="P10" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>21</v>
+      </c>
+      <c r="R10" t="s">
+        <v>21</v>
+      </c>
+      <c r="S10" t="s">
+        <v>21</v>
+      </c>
+      <c r="T10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>990673149</v>
+      </c>
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" t="s">
+        <v>68</v>
+      </c>
+      <c r="F11" t="s">
+        <v>21</v>
+      </c>
+      <c r="G11" t="s">
+        <v>69</v>
+      </c>
+      <c r="H11" t="s">
         <v>24</v>
       </c>
-      <c r="Q8" t="s">
+      <c r="I11" t="s">
+        <v>43</v>
+      </c>
+      <c r="J11">
+        <v>936</v>
+      </c>
+      <c r="K11" t="s">
+        <v>26</v>
+      </c>
+      <c r="L11" t="s">
+        <v>70</v>
+      </c>
+      <c r="M11" t="s">
+        <v>71</v>
+      </c>
+      <c r="N11" t="s">
+        <v>29</v>
+      </c>
+      <c r="O11" t="s">
+        <v>30</v>
+      </c>
+      <c r="P11" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>21</v>
+      </c>
+      <c r="R11" t="s">
+        <v>21</v>
+      </c>
+      <c r="S11" t="s">
+        <v>21</v>
+      </c>
+      <c r="T11" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>990673150</v>
+      </c>
+      <c r="B12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" t="s">
+        <v>68</v>
+      </c>
+      <c r="F12" t="s">
+        <v>21</v>
+      </c>
+      <c r="G12" t="s">
+        <v>69</v>
+      </c>
+      <c r="H12" t="s">
         <v>24</v>
       </c>
-      <c r="R8" t="s">
+      <c r="I12" t="s">
+        <v>43</v>
+      </c>
+      <c r="J12">
+        <v>936</v>
+      </c>
+      <c r="K12" t="s">
+        <v>26</v>
+      </c>
+      <c r="L12" t="s">
+        <v>70</v>
+      </c>
+      <c r="M12" t="s">
+        <v>71</v>
+      </c>
+      <c r="N12" t="s">
+        <v>29</v>
+      </c>
+      <c r="O12" t="s">
+        <v>30</v>
+      </c>
+      <c r="P12" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>21</v>
+      </c>
+      <c r="R12" t="s">
+        <v>21</v>
+      </c>
+      <c r="S12" t="s">
+        <v>21</v>
+      </c>
+      <c r="T12" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>990673151</v>
+      </c>
+      <c r="B13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" t="s">
+        <v>68</v>
+      </c>
+      <c r="F13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G13" t="s">
+        <v>69</v>
+      </c>
+      <c r="H13" t="s">
         <v>24</v>
       </c>
-      <c r="S8" t="s">
+      <c r="I13" t="s">
+        <v>43</v>
+      </c>
+      <c r="J13">
+        <v>936</v>
+      </c>
+      <c r="K13" t="s">
+        <v>26</v>
+      </c>
+      <c r="L13" t="s">
+        <v>70</v>
+      </c>
+      <c r="M13" t="s">
+        <v>71</v>
+      </c>
+      <c r="N13" t="s">
+        <v>29</v>
+      </c>
+      <c r="O13" t="s">
+        <v>30</v>
+      </c>
+      <c r="P13" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>21</v>
+      </c>
+      <c r="R13" t="s">
+        <v>21</v>
+      </c>
+      <c r="S13" t="s">
+        <v>21</v>
+      </c>
+      <c r="T13" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>990740460</v>
+      </c>
+      <c r="B14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" t="s">
+        <v>73</v>
+      </c>
+      <c r="F14" t="s">
+        <v>21</v>
+      </c>
+      <c r="G14" t="s">
+        <v>74</v>
+      </c>
+      <c r="H14" t="s">
         <v>24</v>
       </c>
-      <c r="T8" t="s">
-        <v>47</v>
+      <c r="I14" t="s">
+        <v>75</v>
+      </c>
+      <c r="J14">
+        <v>5824</v>
+      </c>
+      <c r="K14" t="s">
+        <v>26</v>
+      </c>
+      <c r="L14" t="s">
+        <v>76</v>
+      </c>
+      <c r="M14" t="s">
+        <v>77</v>
+      </c>
+      <c r="N14" t="s">
+        <v>29</v>
+      </c>
+      <c r="O14" t="s">
+        <v>30</v>
+      </c>
+      <c r="P14" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>21</v>
+      </c>
+      <c r="R14" t="s">
+        <v>21</v>
+      </c>
+      <c r="S14" t="s">
+        <v>21</v>
+      </c>
+      <c r="T14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>991054690</v>
+      </c>
+      <c r="B15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15" t="s">
+        <v>79</v>
+      </c>
+      <c r="F15" t="s">
+        <v>21</v>
+      </c>
+      <c r="G15" t="s">
+        <v>80</v>
+      </c>
+      <c r="H15" t="s">
+        <v>24</v>
+      </c>
+      <c r="I15" t="s">
+        <v>81</v>
+      </c>
+      <c r="J15">
+        <v>1129</v>
+      </c>
+      <c r="K15" t="s">
+        <v>26</v>
+      </c>
+      <c r="L15" t="s">
+        <v>82</v>
+      </c>
+      <c r="M15" t="s">
+        <v>83</v>
+      </c>
+      <c r="N15" t="s">
+        <v>29</v>
+      </c>
+      <c r="O15" t="s">
+        <v>30</v>
+      </c>
+      <c r="P15" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>21</v>
+      </c>
+      <c r="R15" t="s">
+        <v>21</v>
+      </c>
+      <c r="S15" t="s">
+        <v>21</v>
+      </c>
+      <c r="T15" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>991054691</v>
+      </c>
+      <c r="B16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" t="s">
+        <v>79</v>
+      </c>
+      <c r="F16" t="s">
+        <v>21</v>
+      </c>
+      <c r="G16" t="s">
+        <v>80</v>
+      </c>
+      <c r="H16" t="s">
+        <v>24</v>
+      </c>
+      <c r="I16" t="s">
+        <v>81</v>
+      </c>
+      <c r="J16">
+        <v>1129</v>
+      </c>
+      <c r="K16" t="s">
+        <v>26</v>
+      </c>
+      <c r="L16" t="s">
+        <v>82</v>
+      </c>
+      <c r="M16" t="s">
+        <v>83</v>
+      </c>
+      <c r="N16" t="s">
+        <v>29</v>
+      </c>
+      <c r="O16" t="s">
+        <v>30</v>
+      </c>
+      <c r="P16" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>21</v>
+      </c>
+      <c r="R16" t="s">
+        <v>21</v>
+      </c>
+      <c r="S16" t="s">
+        <v>21</v>
+      </c>
+      <c r="T16" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>991055443</v>
+      </c>
+      <c r="B17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" t="s">
+        <v>20</v>
+      </c>
+      <c r="E17" t="s">
+        <v>85</v>
+      </c>
+      <c r="F17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G17" t="s">
+        <v>86</v>
+      </c>
+      <c r="H17" t="s">
+        <v>24</v>
+      </c>
+      <c r="I17" t="s">
+        <v>87</v>
+      </c>
+      <c r="J17">
+        <v>2658</v>
+      </c>
+      <c r="K17" t="s">
+        <v>26</v>
+      </c>
+      <c r="L17" t="s">
+        <v>88</v>
+      </c>
+      <c r="M17" t="s">
+        <v>89</v>
+      </c>
+      <c r="N17" t="s">
+        <v>29</v>
+      </c>
+      <c r="O17" t="s">
+        <v>30</v>
+      </c>
+      <c r="P17" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>21</v>
+      </c>
+      <c r="R17" t="s">
+        <v>21</v>
+      </c>
+      <c r="S17" t="s">
+        <v>21</v>
+      </c>
+      <c r="T17" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>991057448</v>
+      </c>
+      <c r="B18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" t="s">
+        <v>20</v>
+      </c>
+      <c r="E18" t="s">
+        <v>91</v>
+      </c>
+      <c r="F18" t="s">
+        <v>21</v>
+      </c>
+      <c r="G18" t="s">
+        <v>92</v>
+      </c>
+      <c r="H18" t="s">
+        <v>24</v>
+      </c>
+      <c r="I18" t="s">
+        <v>81</v>
+      </c>
+      <c r="J18">
+        <v>3894</v>
+      </c>
+      <c r="K18" t="s">
+        <v>26</v>
+      </c>
+      <c r="L18" t="s">
+        <v>93</v>
+      </c>
+      <c r="M18" t="s">
+        <v>94</v>
+      </c>
+      <c r="N18" t="s">
+        <v>29</v>
+      </c>
+      <c r="O18" t="s">
+        <v>30</v>
+      </c>
+      <c r="P18" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>21</v>
+      </c>
+      <c r="R18" t="s">
+        <v>21</v>
+      </c>
+      <c r="S18" t="s">
+        <v>21</v>
+      </c>
+      <c r="T18" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:T8">
+  <sortState ref="A2:T18">
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>